<commit_message>
try implement repository pattern
</commit_message>
<xml_diff>
--- a/MetaFiles/DB_Films.xlsx
+++ b/MetaFiles/DB_Films.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\___Code___\__Programing__\EFCoreCodeFirstSample\MetaFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\___Code___\__Programing__\EFCoreCodeFirstSampleWEBAPI\MetaFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F409832-16EA-4B12-8291-89F2D9D24DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6315A3A-E69C-4EB6-9B27-A4FA814D150E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="840" windowWidth="19980" windowHeight="13275" activeTab="5" xr2:uid="{4FE7F364-4D14-4A6C-8063-AF17EB6AC720}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4FE7F364-4D14-4A6C-8063-AF17EB6AC720}"/>
   </bookViews>
   <sheets>
     <sheet name="Films" sheetId="1" r:id="rId1"/>
     <sheet name="Directors" sheetId="5" r:id="rId2"/>
     <sheet name="DirectorList" sheetId="6" r:id="rId3"/>
     <sheet name="Genres" sheetId="3" r:id="rId4"/>
-    <sheet name="GenreList" sheetId="4" r:id="rId5"/>
+    <sheet name="FilmsGenres" sheetId="4" r:id="rId5"/>
     <sheet name="Description" sheetId="2" r:id="rId6"/>
     <sheet name="Users" sheetId="8" r:id="rId7"/>
-    <sheet name="ListFilms" sheetId="7" r:id="rId8"/>
+    <sheet name="FilmsUsers" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -61,9 +61,6 @@
     <t>Бойовик</t>
   </si>
   <si>
-    <t>GenresId</t>
-  </si>
-  <si>
     <t>DirectorName</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>author</t>
+  </si>
+  <si>
+    <t>IdGenres</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -578,7 +578,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -601,10 +601,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -706,7 +706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9B498F-D993-4FA3-9BE0-4B6EFD93C451}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -715,10 +717,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -770,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F158544-647A-4E7B-B371-76879F17D087}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -784,10 +786,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -795,10 +797,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -824,16 +826,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -856,10 +858,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>